<commit_message>
add average of metrics for comparison
</commit_message>
<xml_diff>
--- a/data/fmri/qualitycheck/compare_pipeline/comparepipeline.xlsx
+++ b/data/fmri/qualitycheck/compare_pipeline/comparepipeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Nexus365\Project\pirate_fmri\Analysis\data\fmri\qualitycheck\compare_pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073ACE31-ACC3-430F-A0F1-65BABBFB1D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B8EC31-098B-4609-9EEA-7B774393ED1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>localizer_run1</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>diff_loca</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -510,9 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F33" sqref="A33:F33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1061,6 +1066,27 @@
         <v>0.24880069825297746</v>
       </c>
     </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <f>AVERAGE(A2:A32)</f>
+        <v>0.30578952018269218</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:D33" si="0">AVERAGE(B2:B32)</f>
+        <v>0.28185508600335385</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.21000478231464279</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>0.24726441595827317</v>
+      </c>
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1068,9 +1094,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1718,6 +1746,35 @@
         <v>6.3861088254355848E-4</v>
       </c>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f>AVERAGE(A2:A32)</f>
+        <v>0.18945644311437185</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:F33" si="0">AVERAGE(B2:B32)</f>
+        <v>9.5862533091856619E-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.17806544059893459</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>4.7651877807909935E-4</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.4296041651985284E-3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.0573241779873429E-3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1725,9 +1782,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -2375,6 +2434,35 @@
         <v>1.0055737257432431E-3</v>
       </c>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f>AVERAGE(A2:A32)</f>
+        <v>0.16524060793271864</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:F33" si="0">AVERAGE(B2:B32)</f>
+        <v>7.7231686019357343E-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.17550935287637792</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>5.6725965346146362E-4</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.1308525371640349E-3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.7043524577445303E-3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2382,9 +2470,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -3034,6 +3124,35 @@
         <v>4.3421111790540538E-4</v>
       </c>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f>AVERAGE(A2:A32)</f>
+        <v>0.12093074271676295</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:F33" si="0">AVERAGE(B2:B32)</f>
+        <v>6.7706393277979907E-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.12158014047486848</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>4.3057183124510794E-4</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.1056396367298948E-3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.0389359156588195E-3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3041,9 +3160,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -3693,6 +3814,35 @@
         <v>6.6531276082094589E-4</v>
       </c>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f>AVERAGE(A2:A32)</f>
+        <v>0.12991503073349597</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:F33" si="0">AVERAGE(B2:B32)</f>
+        <v>7.5804935803796325E-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.16067085974788065</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>2.9152274132175133E-4</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.1623319258006568E-3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.4416564157991652E-3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3700,9 +3850,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -4332,6 +4484,61 @@
         <v>1.8719846637567573E-4</v>
       </c>
     </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <f>AVERAGE(A2:A31)</f>
+        <v>0.10669037518203939</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ref="B32:F32" si="0">AVERAGE(B2:B31)</f>
+        <v>7.6202376835930841E-2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0.1171061737053077</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3.4437077724102684E-4</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>8.2497666107579626E-4</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1.1858121461503007E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f>AVERAGE(A2:A32)</f>
+        <v>0.10669037518203937</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:F33" si="1">AVERAGE(B2:B32)</f>
+        <v>7.6202376835930841E-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0.1171061737053077</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>3.4437077724102684E-4</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>8.2497666107579626E-4</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>1.1858121461503007E-3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4339,10 +4546,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5055,6 +5262,12 @@
         <v>4.5241173332923879E-3</v>
       </c>
     </row>
+    <row r="33" spans="6:6">
+      <c r="F33">
+        <f>AVERAGE(F2:F32)</f>
+        <v>3.9195257117855724E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
compare correlation between head motion estimates between pipelines
</commit_message>
<xml_diff>
--- a/data/fmri/qualitycheck/compare_pipeline/comparepipeline.xlsx
+++ b/data/fmri/qualitycheck/compare_pipeline/comparepipeline.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B8EC31-098B-4609-9EEA-7B774393ED1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="mu_XYZdistance" sheetId="2" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="mu_paramdiff-navigation_run3" sheetId="6" r:id="rId5"/>
     <sheet name="mu_paramdiff-navigation_run4" sheetId="7" r:id="rId6"/>
     <sheet name="NMI_of_meanepi" sheetId="8" r:id="rId7"/>
+    <sheet name="mu_corr_betweenpipeline" sheetId="9" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>localizer_run1</t>
   </si>
@@ -166,6 +167,21 @@
   <si>
     <t>mean</t>
   </si>
+  <si>
+    <t>localizer_run1</t>
+  </si>
+  <si>
+    <t>navigation_run1</t>
+  </si>
+  <si>
+    <t>navigation_run2</t>
+  </si>
+  <si>
+    <t>navigation_run3</t>
+  </si>
+  <si>
+    <t>navigation_run4</t>
+  </si>
 </sst>
 </file>
 
@@ -185,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -193,12 +209,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,11 +539,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="5" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="true"/>
+    <col min="2" max="5" width="14.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2">
       <c r="A2">
         <v>0.12159622939937942</v>
       </c>
@@ -559,7 +577,7 @@
         <v>0.28966883961685974</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3">
       <c r="A3">
         <v>0.37236177496205936</v>
       </c>
@@ -576,7 +594,7 @@
         <v>0.30387750388090928</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4">
       <c r="A4">
         <v>0.14637710718863797</v>
       </c>
@@ -593,7 +611,7 @@
         <v>0.22738169822634638</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5">
       <c r="A5">
         <v>0.56850975256211134</v>
       </c>
@@ -610,7 +628,7 @@
         <v>0.38078781899162156</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6">
       <c r="A6">
         <v>0.50103441955075667</v>
       </c>
@@ -627,7 +645,7 @@
         <v>0.30273514216151653</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7">
       <c r="A7">
         <v>0.14514943133551747</v>
       </c>
@@ -644,7 +662,7 @@
         <v>0.10425355289404248</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8">
       <c r="A8">
         <v>0.26998616773889511</v>
       </c>
@@ -661,7 +679,7 @@
         <v>0.14080275138297896</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9">
       <c r="A9">
         <v>9.1084874606551236E-2</v>
       </c>
@@ -678,7 +696,7 @@
         <v>0.10868039275128903</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10">
       <c r="A10">
         <v>0.14868468184574821</v>
       </c>
@@ -695,7 +713,7 @@
         <v>7.6480354904259168E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11">
       <c r="A11">
         <v>0.52975853774695736</v>
       </c>
@@ -712,7 +730,7 @@
         <v>0.54239726951680578</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12">
       <c r="A12">
         <v>0.12617418814048495</v>
       </c>
@@ -729,7 +747,7 @@
         <v>0.2030416644314493</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13">
       <c r="A13">
         <v>0.29723512034955646</v>
       </c>
@@ -746,7 +764,7 @@
         <v>0.27522623243492517</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14">
       <c r="A14">
         <v>0.22505176559816736</v>
       </c>
@@ -763,7 +781,7 @@
         <v>0.25424960208137526</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15">
       <c r="A15">
         <v>0.30713541087776802</v>
       </c>
@@ -780,7 +798,7 @@
         <v>0.17015754796286861</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16">
       <c r="A16">
         <v>0.54611844951922295</v>
       </c>
@@ -797,7 +815,7 @@
         <v>0.17799829494667088</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17">
       <c r="A17">
         <v>0.25347332891462288</v>
       </c>
@@ -814,7 +832,7 @@
         <v>9.4714713854820443E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18">
       <c r="A18">
         <v>0.32448473877952855</v>
       </c>
@@ -831,7 +849,7 @@
         <v>0.21987347217575012</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19">
       <c r="A19">
         <v>0.30449084195158954</v>
       </c>
@@ -848,7 +866,7 @@
         <v>0.11968589422882039</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20">
       <c r="A20">
         <v>0.3804337997433076</v>
       </c>
@@ -865,7 +883,7 @@
         <v>0.12224077466354702</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21">
       <c r="A21">
         <v>0.18093228814139403</v>
       </c>
@@ -882,7 +900,7 @@
         <v>0.20323052287890145</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22">
       <c r="A22">
         <v>0.15736336555621994</v>
       </c>
@@ -899,7 +917,7 @@
         <v>0.10029927845696417</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23">
       <c r="A23">
         <v>0.60598565994572184</v>
       </c>
@@ -916,7 +934,7 @@
         <v>9.5441828481325028E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24">
       <c r="A24">
         <v>0.20102311615013832</v>
       </c>
@@ -933,7 +951,7 @@
         <v>7.6993482574325048E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25">
       <c r="A25">
         <v>0.56256434716642023</v>
       </c>
@@ -950,7 +968,7 @@
         <v>0.18269303245089785</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26">
       <c r="A26">
         <v>9.5161163435396837E-2</v>
       </c>
@@ -967,7 +985,7 @@
         <v>8.9946558173234131E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27">
       <c r="A27">
         <v>1.1526713997052696</v>
       </c>
@@ -984,7 +1002,7 @@
         <v>0.38928853814122144</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28">
       <c r="A28">
         <v>0.24554979554198098</v>
       </c>
@@ -1001,7 +1019,7 @@
         <v>0.1863852883457526</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29">
       <c r="A29">
         <v>0.14577895266809462</v>
       </c>
@@ -1018,7 +1036,7 @@
         <v>0.30216707206195864</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30">
       <c r="A30">
         <v>0.2259933908011045</v>
       </c>
@@ -1035,7 +1053,7 @@
         <v>0.24128920928366504</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31">
       <c r="A31">
         <v>4.2706389223586619E-2</v>
       </c>
@@ -1052,7 +1070,7 @@
         <v>6.0005608126640762E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32">
       <c r="A32">
         <v>0.20460463651726787</v>
       </c>
@@ -1066,7 +1084,7 @@
         <v>0.24880069825297746</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33">
       <c r="A33">
         <f>AVERAGE(A2:A32)</f>
         <v>0.30578952018269218</v>
@@ -1102,11 +1120,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="6" width="15.7265625" customWidth="1"/>
+    <col min="1" max="3" width="13.7265625" customWidth="true"/>
+    <col min="4" max="6" width="15.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1126,7 +1144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>8.4868780809969319E-2</v>
       </c>
@@ -1146,7 +1164,7 @@
         <v>8.003992583004298E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>0.27936574772515327</v>
       </c>
@@ -1166,7 +1184,7 @@
         <v>9.8569906745398796E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>5.906283515E-2</v>
       </c>
@@ -1186,7 +1204,7 @@
         <v>6.5295939875460133E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>0.39534931884417185</v>
       </c>
@@ -1206,7 +1224,7 @@
         <v>1.0530085640941718E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>0.22041299777116569</v>
       </c>
@@ -1226,7 +1244,7 @@
         <v>2.6391402834570552E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>8.412089111245398E-2</v>
       </c>
@@ -1246,7 +1264,7 @@
         <v>1.2157863925119636E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>0.10053338514938648</v>
       </c>
@@ -1266,7 +1284,7 @@
         <v>9.8578127421564414E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>5.3078836205773007E-2</v>
       </c>
@@ -1286,7 +1304,7 @@
         <v>5.3542393807730067E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>0.12004085320116561</v>
       </c>
@@ -1306,7 +1324,7 @@
         <v>8.6635864299363199E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>0.22675497701073624</v>
       </c>
@@ -1326,7 +1344,7 @@
         <v>3.5877239464723924E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>8.0395855695674839E-2</v>
       </c>
@@ -1346,7 +1364,7 @@
         <v>5.070912165923313E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>0.16573310918067488</v>
       </c>
@@ -1366,7 +1384,7 @@
         <v>6.7983183334693247E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>0.21297428076036812</v>
       </c>
@@ -1386,7 +1404,7 @@
         <v>1.1812536282914112E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>0.15828260657046012</v>
       </c>
@@ -1406,7 +1424,7 @@
         <v>1.818890199064417E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>0.30111751505828221</v>
       </c>
@@ -1426,7 +1444,7 @@
         <v>8.8795303098159525E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>0.2309473264217638</v>
       </c>
@@ -1446,7 +1464,7 @@
         <v>1.0277732779947236E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>0.26161740705828224</v>
       </c>
@@ -1466,7 +1484,7 @@
         <v>3.4315637137116561E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>0.26213112765122698</v>
       </c>
@@ -1486,7 +1504,7 @@
         <v>2.148089089791411E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>0.13775790873380364</v>
       </c>
@@ -1506,7 +1524,7 @@
         <v>3.2200713757975458E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>0.12656131139631902</v>
       </c>
@@ -1526,7 +1544,7 @@
         <v>4.3980799904754609E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>8.5518057802760714E-2</v>
       </c>
@@ -1546,7 +1564,7 @@
         <v>2.8689524849441717E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>0.25091119754518409</v>
       </c>
@@ -1566,7 +1584,7 @@
         <v>3.202575819355828E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>0.113379346411227</v>
       </c>
@@ -1586,7 +1604,7 @@
         <v>3.1710554486196326E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>0.42538807976079768</v>
       </c>
@@ -1606,7 +1624,7 @@
         <v>1.0820419438343561E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>5.8116244451533745E-2</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>8.7684060597638055E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>0.97418412007730071</v>
       </c>
@@ -1646,7 +1664,7 @@
         <v>4.1255049876993861E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>4.9089365289570558E-2</v>
       </c>
@@ -1666,7 +1684,7 @@
         <v>5.2858619014601238E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>4.5449797237073632E-2</v>
       </c>
@@ -1686,7 +1704,7 @@
         <v>8.0700785149315961E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>0.14559473149202456</v>
       </c>
@@ -1706,7 +1724,7 @@
         <v>3.7461413147239271E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>3.2173874749168718E-2</v>
       </c>
@@ -1726,7 +1744,7 @@
         <v>5.4844025624907976E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <v>0.13223785022205523</v>
       </c>
@@ -1746,7 +1764,7 @@
         <v>6.3861088254355848E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33">
       <c r="A33">
         <f>AVERAGE(A2:A32)</f>
         <v>0.18945644311437185</v>
@@ -1790,11 +1808,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="6" width="15.7265625" customWidth="1"/>
+    <col min="1" max="3" width="13.7265625" customWidth="true"/>
+    <col min="4" max="6" width="15.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1814,7 +1832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>0.12426529272823648</v>
       </c>
@@ -1834,7 +1852,7 @@
         <v>5.1921624864584449E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>0.19522758413006755</v>
       </c>
@@ -1854,7 +1872,7 @@
         <v>1.0261234069594595E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>5.5151223106827699E-2</v>
       </c>
@@ -1874,7 +1892,7 @@
         <v>2.9406513438310809E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>0.15319995887540538</v>
       </c>
@@ -1894,7 +1912,7 @@
         <v>2.6291037560472971E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>8.7814290411452695E-2</v>
       </c>
@@ -1914,7 +1932,7 @@
         <v>1.2291215407128379E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>3.7909609862304051E-2</v>
       </c>
@@ -1934,7 +1952,7 @@
         <v>2.0064006187287163E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>0.3302141481891892</v>
       </c>
@@ -1954,7 +1972,7 @@
         <v>1.7948896149273647E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>0.16021365112371619</v>
       </c>
@@ -1974,7 +1992,7 @@
         <v>1.5063170579665544E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>7.7248483819932434E-2</v>
       </c>
@@ -1994,7 +2012,7 @@
         <v>6.2641255062871625E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>0.21914866669790542</v>
       </c>
@@ -2014,7 +2032,7 @@
         <v>5.7194085341554066E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>0.27918175905195958</v>
       </c>
@@ -2034,7 +2052,7 @@
         <v>8.9454937952027026E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>0.13729892590489864</v>
       </c>
@@ -2054,7 +2072,7 @@
         <v>5.9329859775101353E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>0.14364314513445947</v>
       </c>
@@ -2074,7 +2092,7 @@
         <v>3.0275288132604731E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>0.21343320056993242</v>
       </c>
@@ -2094,7 +2112,7 @@
         <v>1.9347893593402027E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>0.14191589268393243</v>
       </c>
@@ -2114,7 +2132,7 @@
         <v>1.7889633288344594E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>8.3991982533753395E-2</v>
       </c>
@@ -2134,7 +2152,7 @@
         <v>8.5660626379087845E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>0.14956712276418918</v>
       </c>
@@ -2154,7 +2172,7 @@
         <v>7.1472586797060814E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>6.8042875504391892E-2</v>
       </c>
@@ -2174,7 +2192,7 @@
         <v>2.0530334324999995E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>0.52254478341895272</v>
       </c>
@@ -2194,7 +2212,7 @@
         <v>1.8520010354256759E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>0.40143917552550673</v>
       </c>
@@ -2214,7 +2232,7 @@
         <v>1.206482503547297E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>8.6926835743243253E-2</v>
       </c>
@@ -2234,7 +2252,7 @@
         <v>1.0178344041516893E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>0.19396199854729732</v>
       </c>
@@ -2254,7 +2272,7 @@
         <v>1.4734757645608106E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>4.6059205969594598E-2</v>
       </c>
@@ -2274,7 +2292,7 @@
         <v>2.8470051135447302E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>9.1921562632770265E-2</v>
       </c>
@@ -2294,7 +2312,7 @@
         <v>2.1022875925608112E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>6.2549307755743244E-2</v>
       </c>
@@ -2314,7 +2332,7 @@
         <v>1.1350586318185812E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>0.35669681808108106</v>
       </c>
@@ -2334,7 +2352,7 @@
         <v>3.8149491295945939E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>0.14670401129966218</v>
       </c>
@@ -2354,7 +2372,7 @@
         <v>6.0826101980439187E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>0.22573169143932437</v>
       </c>
@@ -2374,7 +2392,7 @@
         <v>2.9674871422635135E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>0.14113704978449323</v>
       </c>
@@ -2394,7 +2412,7 @@
         <v>3.4352020134422291E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>9.582613062540539E-2</v>
       </c>
@@ -2414,7 +2432,7 @@
         <v>2.1642726523986481E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <v>9.3492461998648649E-2</v>
       </c>
@@ -2434,7 +2452,7 @@
         <v>1.0055737257432431E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33">
       <c r="A33">
         <f>AVERAGE(A2:A32)</f>
         <v>0.16524060793271864</v>
@@ -2478,13 +2496,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="6" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="true"/>
+    <col min="2" max="2" width="14.7265625" customWidth="true"/>
+    <col min="3" max="3" width="13.7265625" customWidth="true"/>
+    <col min="4" max="6" width="15.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2504,7 +2522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>7.1276435094594595E-2</v>
       </c>
@@ -2524,7 +2542,7 @@
         <v>1.4679732243320946E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>0.18684009935976353</v>
       </c>
@@ -2544,7 +2562,7 @@
         <v>2.1461009809219597E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>6.8736062792070965E-2</v>
       </c>
@@ -2564,7 +2582,7 @@
         <v>1.415620758855338E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>6.8237137605067569E-2</v>
       </c>
@@ -2584,7 +2602,7 @@
         <v>5.3906045457128389E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>0.16975197369246622</v>
       </c>
@@ -2604,7 +2622,7 @@
         <v>2.9299094597972974E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>2.1825309095337832E-2</v>
       </c>
@@ -2624,7 +2642,7 @@
         <v>3.8244207416891885E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>3.1962435921351354E-2</v>
       </c>
@@ -2644,7 +2662,7 @@
         <v>7.3076730152770266E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>0.25771289582972973</v>
       </c>
@@ -2664,7 +2682,7 @@
         <v>6.5845905791216217E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>4.1815474012162158E-2</v>
       </c>
@@ -2684,7 +2702,7 @@
         <v>7.6369414162804055E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>0.36033530025574323</v>
       </c>
@@ -2704,7 +2722,7 @@
         <v>7.3954530142972957E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>0.12426749267469592</v>
       </c>
@@ -2724,7 +2742,7 @@
         <v>1.1049144805844592E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>7.3469039261317579E-2</v>
       </c>
@@ -2744,7 +2762,7 @@
         <v>7.9821191811689193E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>0.15609229267341218</v>
       </c>
@@ -2764,7 +2782,7 @@
         <v>3.3856094653064192E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>0.11036169361429053</v>
       </c>
@@ -2784,7 +2802,7 @@
         <v>4.6299832034459455E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>7.7713135026858102E-2</v>
       </c>
@@ -2804,7 +2822,7 @@
         <v>1.067048077952703E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>0.15756730736320945</v>
       </c>
@@ -2824,7 +2842,7 @@
         <v>2.6989870516959462E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>0.26873918239824324</v>
       </c>
@@ -2844,7 +2862,7 @@
         <v>2.9784421147972963E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>5.1846575731081083E-2</v>
       </c>
@@ -2864,7 +2882,7 @@
         <v>1.8895124151756756E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>4.4420022037162152E-2</v>
       </c>
@@ -2884,7 +2902,7 @@
         <v>2.0304018771641894E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>3.4070888618243242E-2</v>
       </c>
@@ -2904,7 +2922,7 @@
         <v>6.2390170354736474E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>6.9742539008418925E-2</v>
       </c>
@@ -2924,7 +2942,7 @@
         <v>3.0891208563074327E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>4.9133283229628379E-2</v>
       </c>
@@ -2944,7 +2962,7 @@
         <v>1.6606948845216214E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>2.3183124460810813E-2</v>
       </c>
@@ -2964,7 +2982,7 @@
         <v>2.487631469088176E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>0.26675994789418928</v>
       </c>
@@ -2984,7 +3002,7 @@
         <v>1.8842658604054055E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>6.7606451241554053E-2</v>
       </c>
@@ -3004,7 +3022,7 @@
         <v>1.7406525001733106E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>0.19406826609858108</v>
       </c>
@@ -3024,7 +3042,7 @@
         <v>2.9667911009527027E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>9.9272734405033772E-2</v>
       </c>
@@ -3044,7 +3062,7 @@
         <v>9.9855568395516912E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>0.16372363353400676</v>
       </c>
@@ -3064,7 +3082,7 @@
         <v>1.1639207191554055E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>0.18624506103341212</v>
       </c>
@@ -3084,7 +3102,7 @@
         <v>8.1250777976060794E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>6.2183323017162152E-2</v>
       </c>
@@ -3104,7 +3122,7 @@
         <v>5.5399549756418923E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <v>0.18989390724005406</v>
       </c>
@@ -3124,7 +3142,7 @@
         <v>4.3421111790540538E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33">
       <c r="A33">
         <f>AVERAGE(A2:A32)</f>
         <v>0.12093074271676295</v>
@@ -3168,13 +3186,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="6" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="true"/>
+    <col min="2" max="2" width="14.7265625" customWidth="true"/>
+    <col min="3" max="3" width="13.7265625" customWidth="true"/>
+    <col min="4" max="6" width="15.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -3194,7 +3212,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>0.17698674841486484</v>
       </c>
@@ -3214,7 +3232,7 @@
         <v>2.5053757474797294E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>0.14765577858337842</v>
       </c>
@@ -3234,7 +3252,7 @@
         <v>3.5629951898195943E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>5.4430645542060792E-2</v>
       </c>
@@ -3254,7 +3272,7 @@
         <v>1.3105918285000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>0.1268490723535135</v>
       </c>
@@ -3274,7 +3292,7 @@
         <v>1.0577496977807431E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>0.26227127433628378</v>
       </c>
@@ -3294,7 +3312,7 @@
         <v>8.5161793647635115E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>7.6881318550506769E-2</v>
       </c>
@@ -3314,7 +3332,7 @@
         <v>3.1398048943783781E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>8.1658501653378374E-2</v>
       </c>
@@ -3334,7 +3352,7 @@
         <v>1.228403116736149E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>0.24801375843741894</v>
       </c>
@@ -3354,7 +3372,7 @@
         <v>4.6104611505067559E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>4.6318136929594599E-2</v>
       </c>
@@ -3374,7 +3392,7 @@
         <v>1.0013008141737841E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>0.12258660428679054</v>
       </c>
@@ -3394,7 +3412,7 @@
         <v>1.1404059672403041E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>0.26678438470357096</v>
       </c>
@@ -3414,7 +3432,7 @@
         <v>1.0736580400033783E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>7.4227190640979712E-2</v>
       </c>
@@ -3434,7 +3452,7 @@
         <v>5.2839385375777026E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>5.3185743694212848E-2</v>
       </c>
@@ -3454,7 +3472,7 @@
         <v>4.7390117356689177E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>6.1780668481351345E-2</v>
       </c>
@@ -3474,7 +3492,7 @@
         <v>1.058968929617061E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>0.17154272852929056</v>
       </c>
@@ -3494,7 +3512,7 @@
         <v>7.0870794731081078E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>2.7783471185202704E-2</v>
       </c>
@@ -3514,7 +3532,7 @@
         <v>6.5480628807297299E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>6.9195216403885165E-2</v>
       </c>
@@ -3534,7 +3552,7 @@
         <v>2.1678729890406076E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>4.4532820806249998E-2</v>
       </c>
@@ -3554,7 +3572,7 @@
         <v>1.8788390009087837E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>0.11922397045878377</v>
       </c>
@@ -3574,7 +3592,7 @@
         <v>3.7773452024628378E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>4.8211357785503374E-2</v>
       </c>
@@ -3594,7 +3612,7 @@
         <v>3.1142114763243252E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>0.17340790923557431</v>
       </c>
@@ -3614,7 +3632,7 @@
         <v>1.9254508618581081E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>0.20342705964999999</v>
       </c>
@@ -3634,7 +3652,7 @@
         <v>3.0950487739222973E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>0.1305787508791216</v>
       </c>
@@ -3654,7 +3672,7 @@
         <v>2.3139719808289187E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>0.14818312305743245</v>
       </c>
@@ -3674,7 +3692,7 @@
         <v>1.2488862828243246E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>0.11271438256418921</v>
       </c>
@@ -3694,7 +3712,7 @@
         <v>1.0456172792162163E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>0.427321945750473</v>
       </c>
@@ -3714,7 +3732,7 @@
         <v>5.568208724530406E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>0.19021016687966213</v>
       </c>
@@ -3734,7 +3752,7 @@
         <v>6.3697193511486495E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>0.11370080442459458</v>
       </c>
@@ -3754,7 +3772,7 @@
         <v>1.2176091007905405E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>6.3273616188648643E-2</v>
       </c>
@@ -3774,7 +3792,7 @@
         <v>2.8599967179143244E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>6.3965785404662162E-2</v>
       </c>
@@ -3794,7 +3812,7 @@
         <v>6.0525399348918918E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <v>0.12046301692719594</v>
       </c>
@@ -3814,7 +3832,7 @@
         <v>6.6531276082094589E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33">
       <c r="A33">
         <f>AVERAGE(A2:A32)</f>
         <v>0.12991503073349597</v>
@@ -3858,13 +3876,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="6" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="true"/>
+    <col min="2" max="2" width="14.7265625" customWidth="true"/>
+    <col min="3" max="3" width="13.7265625" customWidth="true"/>
+    <col min="4" max="6" width="15.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -3884,7 +3902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>0.17320697950000002</v>
       </c>
@@ -3904,7 +3922,7 @@
         <v>5.6557210966216213E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>0.17659265375472971</v>
       </c>
@@ -3924,7 +3942,7 @@
         <v>1.7764323372027031E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>0.11019145815266893</v>
       </c>
@@ -3944,7 +3962,7 @@
         <v>9.0107705354054051E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>0.31522292630540538</v>
       </c>
@@ -3964,7 +3982,7 @@
         <v>6.8994653801351361E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>0.21214476612297298</v>
       </c>
@@ -3984,7 +4002,7 @@
         <v>8.974683497037164E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>6.8654507854054053E-2</v>
       </c>
@@ -4004,7 +4022,7 @@
         <v>9.1024907419864849E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>3.7821938457432425E-2</v>
       </c>
@@ -4024,7 +4042,7 @@
         <v>2.3279028521486487E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>6.806131577736485E-2</v>
       </c>
@@ -4044,7 +4062,7 @@
         <v>9.5450397386250018E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>3.5370297683070949E-2</v>
       </c>
@@ -4064,7 +4082,7 @@
         <v>6.0407688663374997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>0.110425581225</v>
       </c>
@@ -4084,7 +4102,7 @@
         <v>1.9726043665844596E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>0.18296036390270273</v>
       </c>
@@ -4104,7 +4122,7 @@
         <v>1.7083853642128378E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>0.18725620038614868</v>
       </c>
@@ -4124,7 +4142,7 @@
         <v>7.098893182263512E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>9.7430562686824346E-2</v>
       </c>
@@ -4144,7 +4162,7 @@
         <v>2.3478303266081077E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>0.13143884707819598</v>
       </c>
@@ -4164,7 +4182,7 @@
         <v>8.0247763631756744E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>3.2672805584121618E-2</v>
       </c>
@@ -4184,7 +4202,7 @@
         <v>1.0623140354050675E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>4.0240832896959455E-2</v>
       </c>
@@ -4204,7 +4222,7 @@
         <v>8.5713467098817568E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>0.19448736460506758</v>
       </c>
@@ -4224,7 +4242,7 @@
         <v>2.4112780069695944E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>8.8192917268141893E-2</v>
       </c>
@@ -4244,7 +4262,7 @@
         <v>9.8786448546959448E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>8.3943109580743261E-2</v>
       </c>
@@ -4264,7 +4282,7 @@
         <v>4.9481254523165536E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>6.9263438811486472E-2</v>
       </c>
@@ -4284,7 +4302,7 @@
         <v>5.0104038398885136E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>1.7961347636486484E-2</v>
       </c>
@@ -4304,7 +4322,7 @@
         <v>2.9455807449108105E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>7.8746111281081096E-2</v>
       </c>
@@ -4324,7 +4342,7 @@
         <v>2.0169771711013515E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>1.5164678909493242E-2</v>
       </c>
@@ -4344,7 +4362,7 @@
         <v>1.1109722473875E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>0.14892564776042905</v>
       </c>
@@ -4364,7 +4382,7 @@
         <v>4.5484232400135142E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>5.2040571087094589E-2</v>
       </c>
@@ -4384,7 +4402,7 @@
         <v>8.8252223773648637E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>0.20274436113668923</v>
       </c>
@@ -4404,7 +4422,7 @@
         <v>6.5853462556300672E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>0.14567516708266892</v>
       </c>
@@ -4424,7 +4442,7 @@
         <v>8.8723633273486496E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>4.21155531827027E-2</v>
       </c>
@@ -4444,7 +4462,7 @@
         <v>3.4445981471591211E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>6.7955302988277039E-2</v>
       </c>
@@ -4464,7 +4482,7 @@
         <v>1.0356933490677026E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>1.3803646763168923E-2</v>
       </c>
@@ -4484,7 +4502,7 @@
         <v>1.8719846637567573E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <f>AVERAGE(A2:A31)</f>
         <v>0.10669037518203939</v>
@@ -4510,7 +4528,7 @@
         <v>1.1858121461503007E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33">
       <c r="A33">
         <f>AVERAGE(A2:A32)</f>
         <v>0.10669037518203937</v>
@@ -4548,19 +4566,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" customWidth="true"/>
+    <col min="2" max="2" width="19.7265625" customWidth="true"/>
+    <col min="3" max="3" width="17.81640625" customWidth="true"/>
+    <col min="4" max="4" width="17.90625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -4580,7 +4598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>1.028583342586084</v>
       </c>
@@ -4602,7 +4620,7 @@
         <v>2.4556564922990631E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>1.0254782474863995</v>
       </c>
@@ -4624,7 +4642,7 @@
         <v>2.7915088291317058E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>1.0271095274269417</v>
       </c>
@@ -4646,7 +4664,7 @@
         <v>1.6808672254524648E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>1.0256723548154596</v>
       </c>
@@ -4668,7 +4686,7 @@
         <v>3.4475444823709456E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>1.0290498983462106</v>
       </c>
@@ -4690,7 +4708,7 @@
         <v>4.2074554896511795E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>1.0266111317465672</v>
       </c>
@@ -4712,7 +4730,7 @@
         <v>3.2793637364749717E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>1.0286333797752998</v>
       </c>
@@ -4734,7 +4752,7 @@
         <v>4.7253953293995288E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>1.0287333646110099</v>
       </c>
@@ -4756,7 +4774,7 @@
         <v>5.2074262633210466E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>1.0261295953590719</v>
       </c>
@@ -4778,7 +4796,7 @@
         <v>3.0149987417700252E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>1.0281845589672862</v>
       </c>
@@ -4800,7 +4818,7 @@
         <v>5.0990348035062638E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>1.0278654533063389</v>
       </c>
@@ -4822,7 +4840,7 @@
         <v>4.3248555361026231E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>1.0305814044051389</v>
       </c>
@@ -4844,7 +4862,7 @@
         <v>5.0573863154483867E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>1.0278792108715524</v>
       </c>
@@ -4866,7 +4884,7 @@
         <v>3.2649358344063462E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>1.0283444061177116</v>
       </c>
@@ -4888,7 +4906,7 @@
         <v>4.291286427230645E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>1.0281140977255161</v>
       </c>
@@ -4910,7 +4928,7 @@
         <v>4.5719119603939706E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>1.0294309672434474</v>
       </c>
@@ -4932,7 +4950,7 @@
         <v>5.0310926420464863E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>1.0272713812600498</v>
       </c>
@@ -4954,7 +4972,7 @@
         <v>3.2710320971465201E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>1.0276230829447583</v>
       </c>
@@ -4976,7 +4994,7 @@
         <v>3.5162190610080746E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>1.0264828600731446</v>
       </c>
@@ -4998,7 +5016,7 @@
         <v>4.0435100902953547E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>1.0269685611860047</v>
       </c>
@@ -5020,7 +5038,7 @@
         <v>2.5169791978711942E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>1.029592040921353</v>
       </c>
@@ -5042,7 +5060,7 @@
         <v>4.8629800532644651E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>1.0269646325810855</v>
       </c>
@@ -5064,7 +5082,7 @@
         <v>4.1182892507367619E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>1.0263723620287011</v>
       </c>
@@ -5086,7 +5104,7 @@
         <v>3.4179338637536638E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>1.0267702895743471</v>
       </c>
@@ -5108,7 +5126,7 @@
         <v>4.1899671474681099E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>1.0260776605000452</v>
       </c>
@@ -5130,7 +5148,7 @@
         <v>4.0728234670321939E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>1.0267634918867006</v>
       </c>
@@ -5152,7 +5170,7 @@
         <v>5.8011153741863719E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>1.0270458114323284</v>
       </c>
@@ -5174,7 +5192,7 @@
         <v>2.7245007345018113E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>1.0289942469343174</v>
       </c>
@@ -5196,7 +5214,7 @@
         <v>4.6285784070028146E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>1.0279671069851457</v>
       </c>
@@ -5218,7 +5236,7 @@
         <v>3.8324282530659559E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>1.0265782364509894</v>
       </c>
@@ -5240,7 +5258,7 @@
         <v>3.5341026257214025E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <v>1.0266403080895312</v>
       </c>
@@ -5262,7 +5280,7 @@
         <v>4.5241173332923879E-3</v>
       </c>
     </row>
-    <row r="33" spans="6:6">
+    <row r="33">
       <c r="F33">
         <f>AVERAGE(F2:F32)</f>
         <v>3.9195257117855724E-3</v>
@@ -5271,4 +5289,562 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E32"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.89453125" customWidth="true"/>
+    <col min="2" max="2" width="14.7109375" customWidth="true"/>
+    <col min="3" max="3" width="14.7109375" customWidth="true"/>
+    <col min="4" max="4" width="14.7109375" customWidth="true"/>
+    <col min="5" max="5" width="14.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0.90523402536837461</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.93103812780776485</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.93670899074615832</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.93495445530002963</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.8483251000678399</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>0.81741553583617799</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.93364718054529938</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0.92103931645034542</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.90094302340126597</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.70003227302245596</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>0.85711335151020629</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0.79302823216488505</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0.7906682656344034</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0.75879447098107999</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0.9313554084632053</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>0.77539736968200013</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0.81644544176495071</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.80492763541172774</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.93246209452189532</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0.86574947102563826</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>0.86386534102078139</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0.88441676528650304</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0.91940225078236548</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0.75121679541862196</v>
+      </c>
+      <c r="E6" s="0">
+        <v>0.91116363804150868</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>0.82941867731893837</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0.96261857978039389</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0.87268397014809196</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0.80826401389678215</v>
+      </c>
+      <c r="E7" s="0">
+        <v>0.9491529666366515</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>0.89581512199809277</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0.98650313291773195</v>
+      </c>
+      <c r="C8" s="0">
+        <v>0.9687870698893617</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0.81199043848578734</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.93512846965213159</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>0.90162506650108665</v>
+      </c>
+      <c r="B9" s="0">
+        <v>0.95779953192802758</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.96575522054213814</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.79513377780344729</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0.8880393764874519</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>0.96074126237836033</v>
+      </c>
+      <c r="B10" s="0">
+        <v>0.96065258332376346</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0.95492281620348962</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.95991430414474566</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.97025381289663681</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>0.84100353221343027</v>
+      </c>
+      <c r="B11" s="0">
+        <v>0.98346627038161205</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0.96928508172958772</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0.75312926310674078</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0.76347713763627778</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>0.95516485305675547</v>
+      </c>
+      <c r="B12" s="0">
+        <v>0.86055942615832326</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0.98047229561352245</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0.80572905437655296</v>
+      </c>
+      <c r="E12" s="0">
+        <v>0.98273007629405607</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>0.87117641452883954</v>
+      </c>
+      <c r="B13" s="0">
+        <v>0.95559848655399204</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0.90855425336119255</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0.96423975019775587</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0.95006780156973125</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>0.99193607226396407</v>
+      </c>
+      <c r="B14" s="0">
+        <v>0.91594166058080939</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0.91275827583457991</v>
+      </c>
+      <c r="D14" s="0">
+        <v>0.84319454091851576</v>
+      </c>
+      <c r="E14" s="0">
+        <v>0.91231435047159726</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>0.91176668536613958</v>
+      </c>
+      <c r="B15" s="0">
+        <v>0.88563035864098139</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0.93065168255763708</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0.90103921867139469</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0.93972271046506395</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>0.84205804804609885</v>
+      </c>
+      <c r="B16" s="0">
+        <v>0.95621244061009802</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0.90210146105970901</v>
+      </c>
+      <c r="D16" s="0">
+        <v>0.94214980314385011</v>
+      </c>
+      <c r="E16" s="0">
+        <v>0.85841494483109271</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>0.98644873273086719</v>
+      </c>
+      <c r="B17" s="0">
+        <v>0.9702698894116244</v>
+      </c>
+      <c r="C17" s="0">
+        <v>0.69492388159736718</v>
+      </c>
+      <c r="D17" s="0">
+        <v>0.89931547584187255</v>
+      </c>
+      <c r="E17" s="0">
+        <v>0.87410898243099233</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>0.91326018466671821</v>
+      </c>
+      <c r="B18" s="0">
+        <v>0.77506682824137962</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0.87777669888286791</v>
+      </c>
+      <c r="D18" s="0">
+        <v>0.93598812522493768</v>
+      </c>
+      <c r="E18" s="0">
+        <v>0.93355860086095488</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>0.9831857104495475</v>
+      </c>
+      <c r="B19" s="0">
+        <v>0.94447740241495326</v>
+      </c>
+      <c r="C19" s="0">
+        <v>0.98643180228018901</v>
+      </c>
+      <c r="D19" s="0">
+        <v>0.97465021305365163</v>
+      </c>
+      <c r="E19" s="0">
+        <v>0.99598734664103772</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>0.98078026748368385</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0.9258225187648369</v>
+      </c>
+      <c r="C20" s="0">
+        <v>0.96716911942822392</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0.91504879981238252</v>
+      </c>
+      <c r="E20" s="0">
+        <v>0.94601601149133696</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>0.81798441395553712</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0.94320102052818877</v>
+      </c>
+      <c r="C21" s="0">
+        <v>0.94074017633770213</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0.97019296031916558</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0.95448778488857899</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>0.98559766618395928</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0.96908561012320182</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0.97291973188280423</v>
+      </c>
+      <c r="D22" s="0">
+        <v>0.92913681058233133</v>
+      </c>
+      <c r="E22" s="0">
+        <v>0.939251596065656</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>0.89404159049486942</v>
+      </c>
+      <c r="B23" s="0">
+        <v>0.96330253932596754</v>
+      </c>
+      <c r="C23" s="0">
+        <v>0.99422275104092084</v>
+      </c>
+      <c r="D23" s="0">
+        <v>0.94103426890810271</v>
+      </c>
+      <c r="E23" s="0">
+        <v>0.95730017880441254</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>0.86966604673157188</v>
+      </c>
+      <c r="B24" s="0">
+        <v>0.84437795437969754</v>
+      </c>
+      <c r="C24" s="0">
+        <v>0.72940503673799684</v>
+      </c>
+      <c r="D24" s="0">
+        <v>0.80820859225251285</v>
+      </c>
+      <c r="E24" s="0">
+        <v>0.90021162826114154</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>0.96105328271990997</v>
+      </c>
+      <c r="B25" s="0">
+        <v>0.89553845343079785</v>
+      </c>
+      <c r="C25" s="0">
+        <v>0.98758803306926257</v>
+      </c>
+      <c r="D25" s="0">
+        <v>0.83259219354026703</v>
+      </c>
+      <c r="E25" s="0">
+        <v>0.87344067446243878</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>0.88336382131965729</v>
+      </c>
+      <c r="B26" s="0">
+        <v>0.96326552157528411</v>
+      </c>
+      <c r="C26" s="0">
+        <v>0.95940662887566119</v>
+      </c>
+      <c r="D26" s="0">
+        <v>0.85230722741729192</v>
+      </c>
+      <c r="E26" s="0">
+        <v>0.95865708401332028</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>0.88672608094223604</v>
+      </c>
+      <c r="B27" s="0">
+        <v>0.96224382672105258</v>
+      </c>
+      <c r="C27" s="0">
+        <v>0.91251163026896231</v>
+      </c>
+      <c r="D27" s="0">
+        <v>0.88976625788248276</v>
+      </c>
+      <c r="E27" s="0">
+        <v>0.91946152443147289</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>0.90754233369191473</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0.97378706125192716</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0.96556987170140174</v>
+      </c>
+      <c r="D28" s="0">
+        <v>0.94814510880271774</v>
+      </c>
+      <c r="E28" s="0">
+        <v>0.98135121730807373</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>0.97633816360757708</v>
+      </c>
+      <c r="B29" s="0">
+        <v>0.89132762150552092</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0.93326692924720878</v>
+      </c>
+      <c r="D29" s="0">
+        <v>0.88114984477095548</v>
+      </c>
+      <c r="E29" s="0">
+        <v>0.72596827092818528</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>0.89978307146127134</v>
+      </c>
+      <c r="B30" s="0">
+        <v>0.92951377902940335</v>
+      </c>
+      <c r="C30" s="0">
+        <v>0.91832411722264695</v>
+      </c>
+      <c r="D30" s="0">
+        <v>0.9139380697941113</v>
+      </c>
+      <c r="E30" s="0">
+        <v>0.8262827988219158</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>0.96391717412054601</v>
+      </c>
+      <c r="B31" s="0">
+        <v>0.74787584288691544</v>
+      </c>
+      <c r="C31" s="0">
+        <v>0.75068386930981701</v>
+      </c>
+      <c r="D31" s="0">
+        <v>0.89684133167134883</v>
+      </c>
+      <c r="E31" s="0">
+        <v>0.97534926870151761</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>0.87385812848232458</v>
+      </c>
+      <c r="B32" s="0">
+        <v>0.93425008879885063</v>
+      </c>
+      <c r="C32" s="0">
+        <v>0.90157045144743542</v>
+      </c>
+      <c r="D32" s="0">
+        <v>0.91124645631057721</v>
+      </c>
+      <c r="E32" s="0"/>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>